<commit_message>
Single / double hour lessons, daarnaast facilities inlezen uit input en opslaan
</commit_message>
<xml_diff>
--- a/inputs/vakkenurenaantallen.xlsx
+++ b/inputs/vakkenurenaantallen.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="42">
   <si>
     <t>urenH1</t>
   </si>
@@ -121,6 +121,30 @@
   </si>
   <si>
     <t>FA</t>
+  </si>
+  <si>
+    <t>H1|1C|1C</t>
+  </si>
+  <si>
+    <t>V1|1C|1C</t>
+  </si>
+  <si>
+    <t>H1|1ALG|1ALG</t>
+  </si>
+  <si>
+    <t>V1|1ALG|1ALG</t>
+  </si>
+  <si>
+    <t>H2|1ALG|1ALG</t>
+  </si>
+  <si>
+    <t>V2|1ALG|1ALG</t>
+  </si>
+  <si>
+    <t>H3|1ALG|1ALG</t>
+  </si>
+  <si>
+    <t>V3|1ALG|1ALG</t>
   </si>
 </sst>
 </file>
@@ -492,10 +516,18 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -525,22 +557,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -548,22 +580,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -571,22 +603,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -597,19 +629,19 @@
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
         <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
         <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -620,19 +652,19 @@
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s">
         <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -663,22 +695,22 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -686,22 +718,22 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -709,22 +741,22 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -732,22 +764,22 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -755,22 +787,22 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G12" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -784,16 +816,16 @@
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -807,16 +839,16 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G14" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -824,10 +856,10 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
         <v>26</v>
@@ -847,22 +879,22 @@
         <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G16" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>